<commit_message>
End-to-end test script added
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/ExcelReader.xlsx
+++ b/src/test/resources/testData/ExcelReader.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>user</t>
   </si>
@@ -44,6 +44,12 @@
   </si>
   <si>
     <t>visual_user</t>
+  </si>
+  <si>
+    <t>Manthan</t>
+  </si>
+  <si>
+    <t>Mali</t>
   </si>
 </sst>
 </file>
@@ -392,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,6 +452,21 @@
         <v>9</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>416410</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>